<commit_message>
Activities & GiftLogs Completed - 16th June 2023
</commit_message>
<xml_diff>
--- a/TestData/T1523_GiftLog_ApproveGifts_DefaultLayoutFieldsAndFieldsValues.xlsx
+++ b/TestData/T1523_GiftLog_ApproveGifts_DefaultLayoutFieldsAndFieldsValues.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngoyal0630\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779485D4-D110-48FC-AC1A-EB389E9AFA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2970" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Client Gift Pre-approval</t>
   </si>
@@ -42,9 +43,6 @@
     <t>Charitable Contribution</t>
   </si>
   <si>
-    <t>100.00</t>
-  </si>
-  <si>
     <t>GiftValue</t>
   </si>
   <si>
@@ -154,15 +152,12 @@
   </si>
   <si>
     <t>Gift Value</t>
-  </si>
-  <si>
-    <t>110.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,9 +210,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -498,40 +493,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
     </row>
   </sheetData>
@@ -541,81 +536,81 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" t="s">
         <v>36</v>
-      </c>
-      <c r="G2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -624,115 +619,115 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="240" x14ac:dyDescent="0.25">
+      <c r="O1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -742,23 +737,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>